<commit_message>
updated all reduced-form tables for data till july 2022
</commit_message>
<xml_diff>
--- a/workingfolder/tables/InfExpSPFDstSum.xlsx
+++ b/workingfolder/tables/InfExpSPFDstSum.xlsx
@@ -64,7 +64,7 @@
   <sheetData>
     <row r="2">
       <c r="B2" s="0">
-        <v>2141</v>
+        <v>2248</v>
       </c>
       <c r="C2" s="0">
         <v>-5</v>
@@ -73,22 +73,22 @@
         <v>0.32200178888157344</v>
       </c>
       <c r="E2" s="0">
-        <v>1.2500487123242476</v>
+        <v>1.2754543869888129</v>
       </c>
       <c r="F2" s="0">
-        <v>1.7499695121417975</v>
+        <v>1.7499930404196875</v>
       </c>
       <c r="G2" s="0">
-        <v>2.0035519067321754</v>
+        <v>2.0324273573703286</v>
       </c>
       <c r="H2" s="0">
-        <v>2.2698175049884339</v>
+        <v>2.3155170360995099</v>
       </c>
       <c r="I2" s="0">
-        <v>2.5999371169863359</v>
+        <v>2.8803168627721134</v>
       </c>
       <c r="J2" s="0">
-        <v>4.4975269684888906</v>
+        <v>7</v>
       </c>
       <c r="K2" s="0">
         <v>7</v>
@@ -96,63 +96,63 @@
     </row>
     <row r="3">
       <c r="B3" s="0">
-        <v>2108</v>
+        <v>2215</v>
       </c>
       <c r="C3" s="0">
         <v>-5</v>
       </c>
       <c r="D3" s="0">
-        <v>0.50000836261783843</v>
+        <v>0.50000914647851735</v>
       </c>
       <c r="E3" s="0">
-        <v>1.4999849072773597</v>
+        <v>1.5</v>
       </c>
       <c r="F3" s="0">
-        <v>1.8104820237171761</v>
+        <v>1.8237591310066081</v>
       </c>
       <c r="G3" s="0">
-        <v>2.0985116017597667</v>
+        <v>2.1121569147346007</v>
       </c>
       <c r="H3" s="0">
-        <v>2.3056604005526644</v>
+        <v>2.3476674993423572</v>
       </c>
       <c r="I3" s="0">
-        <v>2.6127169663954684</v>
+        <v>2.7197624917577548</v>
       </c>
       <c r="J3" s="0">
-        <v>3.2498641183399615</v>
+        <v>3.7398706907842594</v>
       </c>
       <c r="K3" s="0">
-        <v>4.3480249755672737</v>
+        <v>5.4504432625421222</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="0">
-        <v>2021</v>
+        <v>2126</v>
       </c>
       <c r="C4" s="0">
         <v>-0.6410755134127748</v>
       </c>
       <c r="D4" s="0">
-        <v>0.54572289678554498</v>
+        <v>0.5530453843261991</v>
       </c>
       <c r="E4" s="0">
-        <v>1.2043302978755213</v>
+        <v>1.2391600252454147</v>
       </c>
       <c r="F4" s="0">
-        <v>1.4999994679089177</v>
+        <v>1.5</v>
       </c>
       <c r="G4" s="0">
-        <v>1.7988042993516358</v>
+        <v>1.8198101949859684</v>
       </c>
       <c r="H4" s="0">
-        <v>2.1001940303488711</v>
+        <v>2.1747870311313684</v>
       </c>
       <c r="I4" s="0">
-        <v>2.3831413993546495</v>
+        <v>2.6703170754544416</v>
       </c>
       <c r="J4" s="0">
-        <v>4.231596326534917</v>
+        <v>5.8074698438851211</v>
       </c>
       <c r="K4" s="0">
         <v>7</v>
@@ -160,39 +160,39 @@
     </row>
     <row r="5">
       <c r="B5" s="0">
-        <v>1998</v>
+        <v>2103</v>
       </c>
       <c r="C5" s="0">
         <v>-0.97881257239559516</v>
       </c>
       <c r="D5" s="0">
-        <v>0.59473746783291404</v>
+        <v>0.607599351679037</v>
       </c>
       <c r="E5" s="0">
-        <v>1.3504950327821161</v>
+        <v>1.3710995797407459</v>
       </c>
       <c r="F5" s="0">
-        <v>1.6880265224966038</v>
+        <v>1.7005584140972005</v>
       </c>
       <c r="G5" s="0">
-        <v>1.9361736448599074</v>
+        <v>1.961975970462243</v>
       </c>
       <c r="H5" s="0">
-        <v>2.1801898050140318</v>
+        <v>2.2244838230531681</v>
       </c>
       <c r="I5" s="0">
-        <v>2.4110812014698335</v>
+        <v>2.5324273573703286</v>
       </c>
       <c r="J5" s="0">
-        <v>3.1237891369684494</v>
+        <v>3.6353338606646077</v>
       </c>
       <c r="K5" s="0">
-        <v>4.1761185770238756</v>
+        <v>4.3384779853175885</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" s="0">
-        <v>2141</v>
+        <v>2248</v>
       </c>
       <c r="C6" s="0">
         <v>0.00018752649471832244</v>
@@ -201,22 +201,22 @@
         <v>0.01728085867382223</v>
       </c>
       <c r="E6" s="0">
-        <v>0.03408898422851428</v>
+        <v>0.034088984228514287</v>
       </c>
       <c r="F6" s="0">
-        <v>0.063688381130907357</v>
+        <v>0.064910316716484562</v>
       </c>
       <c r="G6" s="0">
-        <v>0.10557814235753817</v>
+        <v>0.10952298905653934</v>
       </c>
       <c r="H6" s="0">
-        <v>0.21497738041080047</v>
+        <v>0.2227019704819278</v>
       </c>
       <c r="I6" s="0">
-        <v>0.34926288550712503</v>
+        <v>0.39011374829700596</v>
       </c>
       <c r="J6" s="0">
-        <v>1.5373219723242146</v>
+        <v>3</v>
       </c>
       <c r="K6" s="0">
         <v>8.3333333333333339</v>
@@ -224,7 +224,7 @@
     </row>
     <row r="7">
       <c r="B7" s="0">
-        <v>2108</v>
+        <v>2215</v>
       </c>
       <c r="C7" s="0">
         <v>0.00076814672525636065</v>
@@ -233,22 +233,22 @@
         <v>0.027747933524242985</v>
       </c>
       <c r="E7" s="0">
-        <v>0.062456014709564141</v>
+        <v>0.062456014709564252</v>
       </c>
       <c r="F7" s="0">
-        <v>0.088918475003938957</v>
+        <v>0.09191867997209538</v>
       </c>
       <c r="G7" s="0">
-        <v>0.17505410711368374</v>
+        <v>0.18089800617224625</v>
       </c>
       <c r="H7" s="0">
-        <v>0.30514536661545721</v>
+        <v>0.31567240621178039</v>
       </c>
       <c r="I7" s="0">
-        <v>0.56882879093048344</v>
+        <v>0.58600357219994836</v>
       </c>
       <c r="J7" s="0">
-        <v>1.6915462483096027</v>
+        <v>1.7494051723737034</v>
       </c>
       <c r="K7" s="0">
         <v>8.3333333333333339</v>
@@ -256,66 +256,66 @@
     </row>
     <row r="8">
       <c r="B8" s="0">
-        <v>2021</v>
+        <v>2126</v>
       </c>
       <c r="C8" s="0">
-        <v>6.7443202200905453e-07</v>
+        <v>6.7443202200894855e-07</v>
       </c>
       <c r="D8" s="0">
-        <v>0.017280858673822157</v>
+        <v>0.016577477939970681</v>
       </c>
       <c r="E8" s="0">
         <v>0.036445961547596349</v>
       </c>
       <c r="F8" s="0">
-        <v>0.069837823680580072</v>
+        <v>0.06804314145084657</v>
       </c>
       <c r="G8" s="0">
-        <v>0.10649499370618849</v>
+        <v>0.10975849147239662</v>
       </c>
       <c r="H8" s="0">
-        <v>0.21433329073837915</v>
+        <v>0.21896876501691437</v>
       </c>
       <c r="I8" s="0">
-        <v>0.33741659291670978</v>
+        <v>0.35088611195071889</v>
       </c>
       <c r="J8" s="0">
-        <v>1.0941679945211293</v>
+        <v>2.9581809735227602</v>
       </c>
       <c r="K8" s="0">
-        <v>3.4230917174340059</v>
+        <v>5.333333333333333</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="0">
-        <v>1998</v>
+        <v>2103</v>
       </c>
       <c r="C9" s="0">
-        <v>0.017280858673822182</v>
+        <v>0.00076814672525636065</v>
       </c>
       <c r="D9" s="0">
-        <v>0.027747933524242985</v>
+        <v>0.027851138456109308</v>
       </c>
       <c r="E9" s="0">
         <v>0.065682319869217659</v>
       </c>
       <c r="F9" s="0">
-        <v>0.096130881077819447</v>
+        <v>0.10069019199904053</v>
       </c>
       <c r="G9" s="0">
-        <v>0.17627136796214515</v>
+        <v>0.18297995458432156</v>
       </c>
       <c r="H9" s="0">
-        <v>0.29913899947126754</v>
+        <v>0.30589464046892906</v>
       </c>
       <c r="I9" s="0">
-        <v>0.53405999720123509</v>
+        <v>0.55337024156064407</v>
       </c>
       <c r="J9" s="0">
-        <v>1.2277183903189506</v>
+        <v>1.2292561261596213</v>
       </c>
       <c r="K9" s="0">
-        <v>3.0024244356152838</v>
+        <v>2.9716256605973781</v>
       </c>
     </row>
   </sheetData>
@@ -328,21 +328,21 @@
   <sheetData>
     <row r="2">
       <c r="B2" s="0">
-        <v>0.1903028738357595</v>
+        <v>0.19747229553113885</v>
       </c>
       <c r="C2" s="0">
-        <v>0.12915341294868499</v>
+        <v>0.1325881477161438</v>
       </c>
       <c r="D2" s="0">
         <v>0.036445961547596349</v>
       </c>
       <c r="E2" s="0">
-        <v>0.77920421279470886</v>
+        <v>0.81897267744619695</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" s="0">
-        <v>0.19266434935050752</v>
+        <v>0.19262970635355026</v>
       </c>
       <c r="C3" s="0">
         <v>0.11471601138809176</v>
@@ -351,26 +351,26 @@
         <v>0.028548334230126409</v>
       </c>
       <c r="E3" s="0">
-        <v>1.0983148470893038</v>
+        <v>1.0958789974453089</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="0">
-        <v>0.21709504877340147</v>
+        <v>0.22047586011696646</v>
       </c>
       <c r="C4" s="0">
-        <v>0.13931163883266545</v>
+        <v>0.13935924312167314</v>
       </c>
       <c r="D4" s="0">
-        <v>0.027747933524242912</v>
+        <v>0.033299363131445645</v>
       </c>
       <c r="E4" s="0">
-        <v>0.76027543057138047</v>
+        <v>0.76440030548387694</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="0">
-        <v>0.22838098746155824</v>
+        <v>0.22850989966204321</v>
       </c>
       <c r="C5" s="0">
         <v>0.15501789390076606</v>
@@ -379,40 +379,40 @@
         <v>0.034088984228514287</v>
       </c>
       <c r="E5" s="0">
-        <v>0.76003334978379433</v>
+        <v>0.7594737603424776</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" s="0">
-        <v>0.2370543116503398</v>
+        <v>0.24041975576078173</v>
       </c>
       <c r="C6" s="0">
-        <v>0.19058028463594073</v>
+        <v>0.19215573394010094</v>
       </c>
       <c r="D6" s="0">
-        <v>0.027747933524242912</v>
+        <v>0.038069081441861441</v>
       </c>
       <c r="E6" s="0">
-        <v>0.8676519056104075</v>
+        <v>0.8706091364041475</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="0">
-        <v>0.22387155601807307</v>
+        <v>0.22699138659921628</v>
       </c>
       <c r="C7" s="0">
-        <v>0.1756018529082467</v>
+        <v>0.18516105502793523</v>
       </c>
       <c r="D7" s="0">
-        <v>0.027747933524242912</v>
+        <v>0.038069081441861441</v>
       </c>
       <c r="E7" s="0">
-        <v>0.85025814990718473</v>
+        <v>0.85525445387211829</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="0">
-        <v>0.2096011588861057</v>
+        <v>0.21006337023686208</v>
       </c>
       <c r="C8" s="0">
         <v>0.16275651505994099</v>
@@ -421,12 +421,12 @@
         <v>0.034088984228514363</v>
       </c>
       <c r="E8" s="0">
-        <v>0.98402119154578449</v>
+        <v>0.9808870011703118</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="0">
-        <v>0.24357793668801639</v>
+        <v>0.24365800459396564</v>
       </c>
       <c r="C9" s="0">
         <v>0.19302148041709333</v>
@@ -435,12 +435,12 @@
         <v>0.041666666666666664</v>
       </c>
       <c r="E9" s="0">
-        <v>1.0258478859145783</v>
+        <v>1.0295188130124924</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" s="0">
-        <v>0.26021615738098336</v>
+        <v>0.26009620564996405</v>
       </c>
       <c r="C10" s="0">
         <v>0.22262799968288155</v>
@@ -449,54 +449,54 @@
         <v>0.034088984228514287</v>
       </c>
       <c r="E10" s="0">
-        <v>1.0885885032206712</v>
+        <v>1.0878774982011368</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" s="0">
-        <v>0.2506678198104334</v>
+        <v>0.25412507383704214</v>
       </c>
       <c r="C11" s="0">
-        <v>0.19324210039057094</v>
+        <v>0.19971886462871286</v>
       </c>
       <c r="D11" s="0">
-        <v>0.027747933524242912</v>
+        <v>0.033422242066592917</v>
       </c>
       <c r="E11" s="0">
-        <v>1.0749261459826476</v>
+        <v>1.0748983324378134</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" s="0">
-        <v>0.24608664665431129</v>
+        <v>0.24550309451825367</v>
       </c>
       <c r="C12" s="0">
-        <v>0.19207522624664763</v>
+        <v>0.19199474615282092</v>
       </c>
       <c r="D12" s="0">
         <v>0.033422242066592917</v>
       </c>
       <c r="E12" s="0">
-        <v>0.94769527363512229</v>
+        <v>0.94459570598571463</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" s="0">
-        <v>0.2424075194301655</v>
+        <v>0.24412683352942277</v>
       </c>
       <c r="C13" s="0">
         <v>0.16238598230523449</v>
       </c>
       <c r="D13" s="0">
-        <v>0.033422242066592917</v>
+        <v>0.034088984228514169</v>
       </c>
       <c r="E13" s="0">
-        <v>0.93317330025490275</v>
+        <v>0.93008407623201605</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" s="0">
-        <v>0.25494615100678097</v>
+        <v>0.25509911060161738</v>
       </c>
       <c r="C14" s="0">
         <v>0.17742017012156486</v>
@@ -505,7 +505,7 @@
         <v>0.036445961547596349</v>
       </c>
       <c r="E14" s="0">
-        <v>0.92004035476815227</v>
+        <v>0.90734256204267871</v>
       </c>
     </row>
   </sheetData>
@@ -518,167 +518,167 @@
   <sheetData>
     <row r="2">
       <c r="B2" s="0">
-        <v>2100</v>
+        <v>2226</v>
       </c>
       <c r="C2" s="0">
         <v>0.32200178888157344</v>
       </c>
       <c r="D2" s="0">
-        <v>0.63552901231691938</v>
+        <v>0.63754722847946432</v>
       </c>
       <c r="E2" s="0">
-        <v>1.3001700011575821</v>
+        <v>1.3198101949859684</v>
       </c>
       <c r="F2" s="0">
-        <v>1.7499695121417975</v>
+        <v>1.749994787718395</v>
       </c>
       <c r="G2" s="0">
-        <v>2.0036249670386601</v>
+        <v>2.041868400345336</v>
       </c>
       <c r="H2" s="0">
-        <v>2.2594638151136079</v>
+        <v>2.3198101949859682</v>
       </c>
       <c r="I2" s="0">
-        <v>2.5533716262555917</v>
+        <v>2.8986352459131464</v>
       </c>
       <c r="J2" s="0">
-        <v>4.1382758895418856</v>
+        <v>7</v>
       </c>
       <c r="K2" s="0">
-        <v>4.4975269684888906</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" s="0">
-        <v>2065</v>
+        <v>2171</v>
       </c>
       <c r="C3" s="0">
-        <v>0.50000836261783843</v>
+        <v>0.50000914647851735</v>
       </c>
       <c r="D3" s="0">
-        <v>0.81981019498596841</v>
+        <v>0.82620162100876193</v>
       </c>
       <c r="E3" s="0">
-        <v>1.505400966622418</v>
+        <v>1.5334870480978937</v>
       </c>
       <c r="F3" s="0">
-        <v>1.8198101949859684</v>
+        <v>1.8296950781663792</v>
       </c>
       <c r="G3" s="0">
-        <v>2.0970860865331975</v>
+        <v>2.1121569147346007</v>
       </c>
       <c r="H3" s="0">
-        <v>2.3010266211729471</v>
+        <v>2.3409936026018201</v>
       </c>
       <c r="I3" s="0">
-        <v>2.5834831737720103</v>
+        <v>2.6877660814118869</v>
       </c>
       <c r="J3" s="0">
-        <v>3.0877406370663936</v>
+        <v>3.3252251028960185</v>
       </c>
       <c r="K3" s="0">
-        <v>3.2494502552190969</v>
+        <v>3.7398706907842594</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="0">
-        <v>1980</v>
+        <v>2084</v>
       </c>
       <c r="C4" s="0">
-        <v>0.55304536550233763</v>
+        <v>0.56928545361280136</v>
       </c>
       <c r="D4" s="0">
         <v>0.74053618488639228</v>
       </c>
       <c r="E4" s="0">
-        <v>1.2445915206732758</v>
+        <v>1.2499695121417975</v>
       </c>
       <c r="F4" s="0">
-        <v>1.5</v>
+        <v>1.5062422608905204</v>
       </c>
       <c r="G4" s="0">
-        <v>1.7991107348705873</v>
+        <v>1.8198101949859684</v>
       </c>
       <c r="H4" s="0">
-        <v>2.0997554281713442</v>
+        <v>2.1709794348709281</v>
       </c>
       <c r="I4" s="0">
-        <v>2.357189064666982</v>
+        <v>2.565451192145364</v>
       </c>
       <c r="J4" s="0">
-        <v>3.8300656357405489</v>
+        <v>4.4439390779500085</v>
       </c>
       <c r="K4" s="0">
-        <v>4.231596326534917</v>
+        <v>5.8074698438851211</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="0">
-        <v>1958</v>
+        <v>2059</v>
       </c>
       <c r="C5" s="0">
-        <v>0.60091228658748463</v>
+        <v>0.67232708414354347</v>
       </c>
       <c r="D5" s="0">
-        <v>0.84568204655118695</v>
+        <v>0.87285456876589262</v>
       </c>
       <c r="E5" s="0">
-        <v>1.3733389946041503</v>
+        <v>1.3996703019008541</v>
       </c>
       <c r="F5" s="0">
-        <v>1.6966475722976655</v>
+        <v>1.7052985149477167</v>
       </c>
       <c r="G5" s="0">
-        <v>1.9361736448599074</v>
+        <v>1.961975970462243</v>
       </c>
       <c r="H5" s="0">
-        <v>2.1768977538452248</v>
+        <v>2.2134895762999252</v>
       </c>
       <c r="I5" s="0">
-        <v>2.3971351916124535</v>
+        <v>2.4999849072773594</v>
       </c>
       <c r="J5" s="0">
-        <v>2.9013965858777677</v>
+        <v>3.1990732552596279</v>
       </c>
       <c r="K5" s="0">
-        <v>3.0930900549098279</v>
+        <v>3.6332735824220355</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" s="0">
-        <v>2107</v>
+        <v>2229</v>
       </c>
       <c r="C6" s="0">
         <v>0.017280858673822157</v>
       </c>
       <c r="D6" s="0">
-        <v>0.018028461210919413</v>
+        <v>0.018027285569802806</v>
       </c>
       <c r="E6" s="0">
-        <v>0.034088984228514363</v>
+        <v>0.035842887842910405</v>
       </c>
       <c r="F6" s="0">
         <v>0.06567997621544186</v>
       </c>
       <c r="G6" s="0">
-        <v>0.10557814235753817</v>
+        <v>0.11163380205684094</v>
       </c>
       <c r="H6" s="0">
-        <v>0.20582159699651345</v>
+        <v>0.22214677511094608</v>
       </c>
       <c r="I6" s="0">
-        <v>0.33741544539897961</v>
+        <v>0.38803557340855171</v>
       </c>
       <c r="J6" s="0">
-        <v>0.77948996279520577</v>
+        <v>3</v>
       </c>
       <c r="K6" s="0">
-        <v>1.5361097904120442</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="0">
-        <v>2068</v>
+        <v>2174</v>
       </c>
       <c r="C7" s="0">
         <v>0.027747933524242787</v>
@@ -687,30 +687,30 @@
         <v>0.034088984228514169</v>
       </c>
       <c r="E7" s="0">
-        <v>0.062689449759295385</v>
+        <v>0.063688182647057168</v>
       </c>
       <c r="F7" s="0">
-        <v>0.09191867997209538</v>
+        <v>0.092674540896908603</v>
       </c>
       <c r="G7" s="0">
-        <v>0.17432014649075628</v>
+        <v>0.18089800617224625</v>
       </c>
       <c r="H7" s="0">
-        <v>0.29802135586620676</v>
+        <v>0.31052468589714471</v>
       </c>
       <c r="I7" s="0">
-        <v>0.51961095238082999</v>
+        <v>0.53910283975083084</v>
       </c>
       <c r="J7" s="0">
-        <v>1.3136937736957031</v>
+        <v>1.3368341018485699</v>
       </c>
       <c r="K7" s="0">
-        <v>1.6644897291695648</v>
+        <v>1.7364125265249444</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="0">
-        <v>1980</v>
+        <v>2082</v>
       </c>
       <c r="C8" s="0">
         <v>0.017280858673822157</v>
@@ -719,57 +719,57 @@
         <v>0.019540142682291442</v>
       </c>
       <c r="E8" s="0">
-        <v>0.037843882580139807</v>
+        <v>0.038069081441861441</v>
       </c>
       <c r="F8" s="0">
-        <v>0.072278505958867256</v>
+        <v>0.069968228100652702</v>
       </c>
       <c r="G8" s="0">
-        <v>0.10649499370618849</v>
+        <v>0.10975849147239662</v>
       </c>
       <c r="H8" s="0">
-        <v>0.20932203776802805</v>
+        <v>0.21583169994724355</v>
       </c>
       <c r="I8" s="0">
-        <v>0.33230619754862883</v>
+        <v>0.33883041288058452</v>
       </c>
       <c r="J8" s="0">
-        <v>0.72879055483770327</v>
+        <v>0.95443848874753701</v>
       </c>
       <c r="K8" s="0">
-        <v>1.0486858499872631</v>
+        <v>2.9174619646504256</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="0">
-        <v>1967</v>
+        <v>2061</v>
       </c>
       <c r="C9" s="0">
-        <v>0.027747933524242787</v>
+        <v>0.027851138456109308</v>
       </c>
       <c r="D9" s="0">
-        <v>0.033422242066592917</v>
+        <v>0.034088984228514287</v>
       </c>
       <c r="E9" s="0">
-        <v>0.065682319869217659</v>
+        <v>0.068776768518348505</v>
       </c>
       <c r="F9" s="0">
-        <v>0.096130881077819447</v>
+        <v>0.10312517210071119</v>
       </c>
       <c r="G9" s="0">
-        <v>0.17557631517046568</v>
+        <v>0.18297995458432156</v>
       </c>
       <c r="H9" s="0">
-        <v>0.29584117638219104</v>
+        <v>0.30060711093104908</v>
       </c>
       <c r="I9" s="0">
-        <v>0.50567145398969204</v>
+        <v>0.52597333751237019</v>
       </c>
       <c r="J9" s="0">
-        <v>0.98455774420417708</v>
+        <v>0.98931446569207537</v>
       </c>
       <c r="K9" s="0">
-        <v>1.2108241592242479</v>
+        <v>1.2292561261596213</v>
       </c>
     </row>
   </sheetData>
@@ -782,7 +782,7 @@
   <sheetData>
     <row r="2">
       <c r="B2" s="0">
-        <v>2.3239607786384844</v>
+        <v>2.3239952016452992</v>
       </c>
       <c r="C2" s="0">
         <v>2.2994171703895385</v>
@@ -791,12 +791,12 @@
         <v>1.5380241446967706</v>
       </c>
       <c r="E2" s="0">
-        <v>3.0600365815348045</v>
+        <v>3.0599838319237325</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" s="0">
-        <v>2.4005721524555677</v>
+        <v>2.4006086239393332</v>
       </c>
       <c r="C3" s="0">
         <v>2.3473664127208735</v>
@@ -810,7 +810,7 @@
     </row>
     <row r="4">
       <c r="B4" s="0">
-        <v>1.422842326124683</v>
+        <v>1.422660508636753</v>
       </c>
       <c r="C4" s="0">
         <v>1.447241943748155</v>
@@ -824,7 +824,7 @@
     </row>
     <row r="5">
       <c r="B5" s="0">
-        <v>1.2922887596469694</v>
+        <v>1.2921694101727932</v>
       </c>
       <c r="C5" s="0">
         <v>1.2499695121417975</v>
@@ -838,27 +838,27 @@
     </row>
     <row r="6">
       <c r="B6" s="0">
-        <v>1.8716532848681544</v>
+        <v>1.8704425245740466</v>
       </c>
       <c r="C6" s="0">
         <v>1.947241943748155</v>
       </c>
       <c r="D6" s="0">
-        <v>0.76064689333442548</v>
+        <v>0.76075114913859965</v>
       </c>
       <c r="E6" s="0">
-        <v>3.419218761277226</v>
+        <v>3.4192649612241688</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="0">
-        <v>2.031260628293555</v>
+        <v>2.0313038179976224</v>
       </c>
       <c r="C7" s="0">
         <v>2.0029386502459539</v>
       </c>
       <c r="D7" s="0">
-        <v>1.3413603515020451</v>
+        <v>1.3413598224664964</v>
       </c>
       <c r="E7" s="0">
         <v>2.8033542643307361</v>
@@ -866,13 +866,13 @@
     </row>
     <row r="8">
       <c r="B8" s="0">
-        <v>1.853106341083085</v>
+        <v>1.8520629617371256</v>
       </c>
       <c r="C8" s="0">
         <v>1.8289275546248558</v>
       </c>
       <c r="D8" s="0">
-        <v>1.2329214775696999</v>
+        <v>1.2250997977924105</v>
       </c>
       <c r="E8" s="0">
         <v>2.6271128033283424</v>
@@ -880,13 +880,13 @@
     </row>
     <row r="9">
       <c r="B9" s="0">
-        <v>1.8995886804253523</v>
+        <v>1.9005887709911935</v>
       </c>
       <c r="C9" s="0">
         <v>1.9110812014698335</v>
       </c>
       <c r="D9" s="0">
-        <v>1.2526079588120465</v>
+        <v>1.2564101929994531</v>
       </c>
       <c r="E9" s="0">
         <v>2.3848770829038912</v>
@@ -894,13 +894,13 @@
     </row>
     <row r="10">
       <c r="B10" s="0">
-        <v>1.8027993969942635</v>
+        <v>1.8027587207454649</v>
       </c>
       <c r="C10" s="0">
         <v>1.8009228319256256</v>
       </c>
       <c r="D10" s="0">
-        <v>0.71021919351610052</v>
+        <v>0.71023747776524826</v>
       </c>
       <c r="E10" s="0">
         <v>2.3848770829038912</v>
@@ -908,7 +908,7 @@
     </row>
     <row r="11">
       <c r="B11" s="0">
-        <v>2.0401002056102615</v>
+        <v>2.0397140800388471</v>
       </c>
       <c r="C11" s="0">
         <v>2.0682561430582096</v>
@@ -917,15 +917,15 @@
         <v>1.2209829281669435</v>
       </c>
       <c r="E11" s="0">
-        <v>2.5216021875522898</v>
+        <v>2.5215788061400746</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" s="0">
-        <v>2.0460921452961882</v>
+        <v>2.0461058207935978</v>
       </c>
       <c r="C12" s="0">
-        <v>2.0542043653531179</v>
+        <v>2.0541327429629286</v>
       </c>
       <c r="D12" s="0">
         <v>1.5339159156864566</v>
@@ -936,7 +936,7 @@
     </row>
     <row r="13">
       <c r="B13" s="0">
-        <v>2.2955640831947317</v>
+        <v>2.2955318419358139</v>
       </c>
       <c r="C13" s="0">
         <v>2.2553066711205374</v>
@@ -945,12 +945,12 @@
         <v>1.7499930404196875</v>
       </c>
       <c r="E13" s="0">
-        <v>2.9031584443442333</v>
+        <v>2.9030899851256748</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" s="0">
-        <v>2.1769809431897658</v>
+        <v>2.1769687150738024</v>
       </c>
       <c r="C14" s="0">
         <v>2.1469602753265624</v>
@@ -959,7 +959,7 @@
         <v>1.8198101949859684</v>
       </c>
       <c r="E14" s="0">
-        <v>2.9665377149911905</v>
+        <v>2.9668614522861665</v>
       </c>
     </row>
   </sheetData>
@@ -972,7 +972,7 @@
   <sheetData>
     <row r="2">
       <c r="B2" s="0">
-        <v>2.2647241486127361</v>
+        <v>2.2646616624024007</v>
       </c>
       <c r="C2" s="0">
         <v>2.2500011922660725</v>
@@ -981,32 +981,32 @@
         <v>1.6655147703519004</v>
       </c>
       <c r="E2" s="0">
-        <v>2.9978167620746041</v>
+        <v>2.9978966169151753</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" s="0">
-        <v>2.1994740628563623</v>
+        <v>2.2207182389614073</v>
       </c>
       <c r="C3" s="0">
-        <v>2.240827423182008</v>
+        <v>2.2499695121417975</v>
       </c>
       <c r="D3" s="0">
         <v>1</v>
       </c>
       <c r="E3" s="0">
-        <v>3.1494700364804205</v>
+        <v>3.3009730351282753</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="0">
-        <v>1.6330179213093936</v>
+        <v>1.6329913113322516</v>
       </c>
       <c r="C4" s="0">
-        <v>1.6887216022844447</v>
+        <v>1.6893250778540632</v>
       </c>
       <c r="D4" s="0">
-        <v>0.60949664720990437</v>
+        <v>0.60950311897898235</v>
       </c>
       <c r="E4" s="0">
         <v>2.7499930404196875</v>
@@ -1014,27 +1014,27 @@
     </row>
     <row r="5">
       <c r="B5" s="0">
-        <v>1.6348530921791795</v>
+        <v>1.6488690687519612</v>
       </c>
       <c r="C5" s="0">
-        <v>1.6271128033283424</v>
+        <v>1.6299351849533801</v>
       </c>
       <c r="D5" s="0">
-        <v>0.5104897020023309</v>
+        <v>0.51054048083784997</v>
       </c>
       <c r="E5" s="0">
-        <v>2.8904809735012362</v>
+        <v>2.9473200119504641</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" s="0">
-        <v>1.8756124095154465</v>
+        <v>1.8754717661228706</v>
       </c>
       <c r="C6" s="0">
         <v>1.8281668706837988</v>
       </c>
       <c r="D6" s="0">
-        <v>0.82606868005663647</v>
+        <v>0.82620162100876193</v>
       </c>
       <c r="E6" s="0">
         <v>3.0682561430582096</v>
@@ -1042,27 +1042,27 @@
     </row>
     <row r="7">
       <c r="B7" s="0">
-        <v>2.0951164150169079</v>
+        <v>2.0931704397938686</v>
       </c>
       <c r="C7" s="0">
-        <v>2.0727694856313974</v>
+        <v>2.0725549202778439</v>
       </c>
       <c r="D7" s="0">
-        <v>1.3036014597152918</v>
+        <v>1.3035789531335413</v>
       </c>
       <c r="E7" s="0">
-        <v>2.9678490392852126</v>
+        <v>2.9697025850583927</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="0">
-        <v>2.0158012788444615</v>
+        <v>2.017333931130489</v>
       </c>
       <c r="C8" s="0">
         <v>2.0165387844425871</v>
       </c>
       <c r="D8" s="0">
-        <v>1.2526079588120465</v>
+        <v>1.2770051774880544</v>
       </c>
       <c r="E8" s="0">
         <v>2.8033542643307361</v>
@@ -1070,13 +1070,13 @@
     </row>
     <row r="9">
       <c r="B9" s="0">
-        <v>2.0304435463662913</v>
+        <v>2.0310085938482598</v>
       </c>
       <c r="C9" s="0">
-        <v>2.0777389934820505</v>
+        <v>2.0776266807350403</v>
       </c>
       <c r="D9" s="0">
-        <v>1.2526079588120465</v>
+        <v>1.2770051774880544</v>
       </c>
       <c r="E9" s="0">
         <v>2.749995310015362</v>
@@ -1084,13 +1084,13 @@
     </row>
     <row r="10">
       <c r="B10" s="0">
-        <v>2.0180321958311938</v>
+        <v>2.018864549610119</v>
       </c>
       <c r="C10" s="0">
-        <v>2.0000047571922419</v>
+        <v>2.0002169582617069</v>
       </c>
       <c r="D10" s="0">
-        <v>1.392893359163613</v>
+        <v>1.3928933429998991</v>
       </c>
       <c r="E10" s="0">
         <v>2.7403407895183491</v>
@@ -1098,10 +1098,10 @@
     </row>
     <row r="11">
       <c r="B11" s="0">
-        <v>2.1028331335923967</v>
+        <v>2.1028112635573608</v>
       </c>
       <c r="C11" s="0">
-        <v>2.159336517480039</v>
+        <v>2.1593601101812983</v>
       </c>
       <c r="D11" s="0">
         <v>1.4642590643637721</v>
@@ -1112,13 +1112,13 @@
     </row>
     <row r="12">
       <c r="B12" s="0">
-        <v>2.1521240971550837</v>
+        <v>2.1522855914842567</v>
       </c>
       <c r="C12" s="0">
         <v>2.148990384907254</v>
       </c>
       <c r="D12" s="0">
-        <v>1.5433226047401749</v>
+        <v>1.5433091147159372</v>
       </c>
       <c r="E12" s="0">
         <v>2.9633538277045988</v>
@@ -1126,10 +1126,10 @@
     </row>
     <row r="13">
       <c r="B13" s="0">
-        <v>2.3583824404042177</v>
+        <v>2.3584535332089192</v>
       </c>
       <c r="C13" s="0">
-        <v>2.3537590383965941</v>
+        <v>2.355845181943284</v>
       </c>
       <c r="D13" s="0">
         <v>1.8198101949859684</v>
@@ -1140,16 +1140,16 @@
     </row>
     <row r="14">
       <c r="B14" s="0">
-        <v>2.2330671164153513</v>
+        <v>2.2330114754495747</v>
       </c>
       <c r="C14" s="0">
-        <v>2.1889811928390608</v>
+        <v>2.1884529795119887</v>
       </c>
       <c r="D14" s="0">
         <v>1.7446477374882117</v>
       </c>
       <c r="E14" s="0">
-        <v>3.1674762208791756</v>
+        <v>3.1688520637105757</v>
       </c>
     </row>
   </sheetData>
@@ -1162,7 +1162,7 @@
   <sheetData>
     <row r="2">
       <c r="B2" s="0">
-        <v>2.0769385201264789</v>
+        <v>2.0769111294459321</v>
       </c>
       <c r="C2" s="0">
         <v>2.0317349859184191</v>
@@ -1171,12 +1171,12 @@
         <v>1.3594430833850033</v>
       </c>
       <c r="E2" s="0">
-        <v>2.9360301456768827</v>
+        <v>2.9343291453982765</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" s="0">
-        <v>2.2358088625675725</v>
+        <v>2.2357676216267484</v>
       </c>
       <c r="C3" s="0">
         <v>2.2499930404196875</v>
@@ -1185,18 +1185,18 @@
         <v>1.5805108660423635</v>
       </c>
       <c r="E3" s="0">
-        <v>3.1237891369684494</v>
+        <v>3.1239380528319245</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="0">
-        <v>1.4044884437443514</v>
+        <v>1.404246431314266</v>
       </c>
       <c r="C4" s="0">
         <v>1.3473664127208735</v>
       </c>
       <c r="D4" s="0">
-        <v>0.71021919351610052</v>
+        <v>0.71023747776524826</v>
       </c>
       <c r="E4" s="0">
         <v>2.5527580562518448</v>
@@ -1204,13 +1204,13 @@
     </row>
     <row r="5">
       <c r="B5" s="0">
-        <v>1.2558500085008935</v>
+        <v>1.2609908321871652</v>
       </c>
       <c r="C5" s="0">
-        <v>1.2445647686936061</v>
+        <v>1.2499695121417975</v>
       </c>
       <c r="D5" s="0">
-        <v>0.59060503539904685</v>
+        <v>0.62398887103573009</v>
       </c>
       <c r="E5" s="0">
         <v>2.1526270538321559</v>
@@ -1218,7 +1218,7 @@
     </row>
     <row r="6">
       <c r="B6" s="0">
-        <v>1.6557828422376006</v>
+        <v>1.6556878577297856</v>
       </c>
       <c r="C6" s="0">
         <v>1.7194719967058449</v>
@@ -1227,12 +1227,12 @@
         <v>0.74999846943145887</v>
       </c>
       <c r="E6" s="0">
-        <v>2.8812136442924627</v>
+        <v>2.8813648521018065</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="0">
-        <v>1.9134721556364416</v>
+        <v>1.9135060345711064</v>
       </c>
       <c r="C7" s="0">
         <v>1.9204536698776451</v>
@@ -1246,13 +1246,13 @@
     </row>
     <row r="8">
       <c r="B8" s="0">
-        <v>1.6185494857092273</v>
+        <v>1.6190465808254868</v>
       </c>
       <c r="C8" s="0">
         <v>1.5999371169863359</v>
       </c>
       <c r="D8" s="0">
-        <v>0.81965962465973552</v>
+        <v>0.81965962463275477</v>
       </c>
       <c r="E8" s="0">
         <v>2.4677087036951137</v>
@@ -1260,13 +1260,13 @@
     </row>
     <row r="9">
       <c r="B9" s="0">
-        <v>1.7058663910627549</v>
+        <v>1.7058726019610821</v>
       </c>
       <c r="C9" s="0">
         <v>1.692344008811979</v>
       </c>
       <c r="D9" s="0">
-        <v>1.1142323972107753</v>
+        <v>1.1142324181245338</v>
       </c>
       <c r="E9" s="0">
         <v>2.3511868137287477</v>
@@ -1274,13 +1274,13 @@
     </row>
     <row r="10">
       <c r="B10" s="0">
-        <v>1.5237229420269782</v>
+        <v>1.5240051105714416</v>
       </c>
       <c r="C10" s="0">
-        <v>1.4999994679089177</v>
+        <v>1.4998121958142552</v>
       </c>
       <c r="D10" s="0">
-        <v>0.80856161667785476</v>
+        <v>0.80853225087857616</v>
       </c>
       <c r="E10" s="0">
         <v>2.3032950471534757</v>
@@ -1288,13 +1288,13 @@
     </row>
     <row r="11">
       <c r="B11" s="0">
-        <v>1.7391115125747842</v>
+        <v>1.7392158001218212</v>
       </c>
       <c r="C11" s="0">
-        <v>1.75</v>
+        <v>1.7500028282211648</v>
       </c>
       <c r="D11" s="0">
-        <v>0.79867695593342702</v>
+        <v>0.79412804266442727</v>
       </c>
       <c r="E11" s="0">
         <v>2.2918293181181406</v>
@@ -1302,10 +1302,10 @@
     </row>
     <row r="12">
       <c r="B12" s="0">
-        <v>1.8241383204727497</v>
+        <v>1.8241829825509057</v>
       </c>
       <c r="C12" s="0">
-        <v>1.7649418716200498</v>
+        <v>1.7650685010777551</v>
       </c>
       <c r="D12" s="0">
         <v>1.2499695121417975</v>
@@ -1316,13 +1316,13 @@
     </row>
     <row r="13">
       <c r="B13" s="0">
-        <v>2.0670333224635362</v>
+        <v>2.0669583695326073</v>
       </c>
       <c r="C13" s="0">
         <v>2.09591695605714</v>
       </c>
       <c r="D13" s="0">
-        <v>1.5468869080047574</v>
+        <v>1.5442758461948545</v>
       </c>
       <c r="E13" s="0">
         <v>2.5387680006108049</v>
@@ -1330,16 +1330,16 @@
     </row>
     <row r="14">
       <c r="B14" s="0">
-        <v>1.9486740370089093</v>
+        <v>1.9485960436613972</v>
       </c>
       <c r="C14" s="0">
         <v>1.8949856816159851</v>
       </c>
       <c r="D14" s="0">
-        <v>1.4278558225437128</v>
+        <v>1.4277449965225821</v>
       </c>
       <c r="E14" s="0">
-        <v>2.9874152908871272</v>
+        <v>2.9873773095145255</v>
       </c>
     </row>
   </sheetData>
@@ -1352,41 +1352,41 @@
   <sheetData>
     <row r="2">
       <c r="B2" s="0">
-        <v>2.0896380985892549</v>
+        <v>2.0966515010388274</v>
       </c>
       <c r="C2" s="0">
-        <v>2.0887792043421989</v>
+        <v>2.0914168999328546</v>
       </c>
       <c r="D2" s="0">
         <v>1.3606368908444557</v>
       </c>
       <c r="E2" s="0">
-        <v>2.750001602520546</v>
+        <v>2.7994171703895385</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" s="0">
-        <v>2.0679529575203519</v>
+        <v>2.0921338785756989</v>
       </c>
       <c r="C3" s="0">
-        <v>2.1159174567486279</v>
+        <v>2.1271128033283424</v>
       </c>
       <c r="D3" s="0">
         <v>1.052758056251845</v>
       </c>
       <c r="E3" s="0">
-        <v>2.817213229095799</v>
+        <v>3.2550963330108416</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="0">
-        <v>1.5619932177579878</v>
+        <v>1.5705497782397206</v>
       </c>
       <c r="C4" s="0">
-        <v>1.5136041697555251</v>
+        <v>1.5276882387578137</v>
       </c>
       <c r="D4" s="0">
-        <v>0.67813775323576442</v>
+        <v>0.72292964016594141</v>
       </c>
       <c r="E4" s="0">
         <v>2.591971078052723</v>
@@ -1394,13 +1394,13 @@
     </row>
     <row r="5">
       <c r="B5" s="0">
-        <v>1.5371192489533727</v>
+        <v>1.5444216594776887</v>
       </c>
       <c r="C5" s="0">
         <v>1.5</v>
       </c>
       <c r="D5" s="0">
-        <v>0.67237249788858555</v>
+        <v>0.67372301386709399</v>
       </c>
       <c r="E5" s="0">
         <v>2.9000631113645667</v>
@@ -1408,13 +1408,13 @@
     </row>
     <row r="6">
       <c r="B6" s="0">
-        <v>1.7600474358034945</v>
+        <v>1.7599016427414946</v>
       </c>
       <c r="C6" s="0">
         <v>1.750001602520546</v>
       </c>
       <c r="D6" s="0">
-        <v>0.82606868005663647</v>
+        <v>0.82620162100876193</v>
       </c>
       <c r="E6" s="0">
         <v>3.0336795217099537</v>
@@ -1422,10 +1422,10 @@
     </row>
     <row r="7">
       <c r="B7" s="0">
-        <v>1.9733750292738581</v>
+        <v>1.9835083008103476</v>
       </c>
       <c r="C7" s="0">
-        <v>1.9999921875931386</v>
+        <v>1.9999994679089177</v>
       </c>
       <c r="D7" s="0">
         <v>1.2754543869888129</v>
@@ -1436,13 +1436,13 @@
     </row>
     <row r="8">
       <c r="B8" s="0">
-        <v>1.8615858054932168</v>
+        <v>1.8619482875496942</v>
       </c>
       <c r="C8" s="0">
         <v>1.865618823893566</v>
       </c>
       <c r="D8" s="0">
-        <v>1.0490286760583103</v>
+        <v>1.049215262192096</v>
       </c>
       <c r="E8" s="0">
         <v>2.5324273573703286</v>
@@ -1450,7 +1450,7 @@
     </row>
     <row r="9">
       <c r="B9" s="0">
-        <v>1.8820894835883284</v>
+        <v>1.8821081092419591</v>
       </c>
       <c r="C9" s="0">
         <v>1.8632400238838718</v>
@@ -1464,13 +1464,13 @@
     </row>
     <row r="10">
       <c r="B10" s="0">
-        <v>1.8084833917820422</v>
+        <v>1.8085096043783209</v>
       </c>
       <c r="C10" s="0">
-        <v>1.7505300574275648</v>
+        <v>1.7536767309548129</v>
       </c>
       <c r="D10" s="0">
-        <v>1.1788071383305612</v>
+        <v>1.1793841015202573</v>
       </c>
       <c r="E10" s="0">
         <v>2.4730666890462025</v>
@@ -1478,7 +1478,7 @@
     </row>
     <row r="11">
       <c r="B11" s="0">
-        <v>1.8536747166747507</v>
+        <v>1.8536861141001297</v>
       </c>
       <c r="C11" s="0">
         <v>1.8140634234951272</v>
@@ -1492,13 +1492,13 @@
     </row>
     <row r="12">
       <c r="B12" s="0">
-        <v>1.9724450232588957</v>
+        <v>1.9739886822764172</v>
       </c>
       <c r="C12" s="0">
-        <v>1.947241943748155</v>
+        <v>1.9574708886428562</v>
       </c>
       <c r="D12" s="0">
-        <v>1.3283117494240371</v>
+        <v>1.3279496204035142</v>
       </c>
       <c r="E12" s="0">
         <v>2.5396980865210605</v>
@@ -1506,13 +1506,13 @@
     </row>
     <row r="13">
       <c r="B13" s="0">
-        <v>2.1400596999724377</v>
+        <v>2.140041966826665</v>
       </c>
       <c r="C13" s="0">
-        <v>2.1347394830187749</v>
+        <v>2.1297653159767922</v>
       </c>
       <c r="D13" s="0">
-        <v>1.5609217463771352</v>
+        <v>1.5609558613763803</v>
       </c>
       <c r="E13" s="0">
         <v>2.6168541157741072</v>
@@ -1520,16 +1520,16 @@
     </row>
     <row r="14">
       <c r="B14" s="0">
-        <v>2.0091337641109601</v>
+        <v>2.0556644143037524</v>
       </c>
       <c r="C14" s="0">
-        <v>1.9999996000383207</v>
+        <v>1.9999997321677236</v>
       </c>
       <c r="D14" s="0">
-        <v>1.5609217463771352</v>
+        <v>1.5609558613763803</v>
       </c>
       <c r="E14" s="0">
-        <v>2.6046013076222412</v>
+        <v>3.4163063683559036</v>
       </c>
     </row>
   </sheetData>
@@ -1542,7 +1542,7 @@
   <sheetData>
     <row r="2">
       <c r="B2" s="0">
-        <v>0.14156801036787631</v>
+        <v>0.14158452311961436</v>
       </c>
       <c r="C2" s="0">
         <v>0.096130881077819447</v>
@@ -1551,12 +1551,12 @@
         <v>0.022941050441254246</v>
       </c>
       <c r="E2" s="0">
-        <v>0.74761053711215819</v>
+        <v>0.74762882143704779</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" s="0">
-        <v>0.15103470123428367</v>
+        <v>0.1511770330501877</v>
       </c>
       <c r="C3" s="0">
         <v>0.096130881077819252</v>
@@ -1565,26 +1565,26 @@
         <v>0.02227952073088578</v>
       </c>
       <c r="E3" s="0">
-        <v>0.85356769103274377</v>
+        <v>0.84960376725767406</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="0">
-        <v>0.14683567558957356</v>
+        <v>0.15650520000103249</v>
       </c>
       <c r="C4" s="0">
-        <v>0.096130881077819336</v>
+        <v>0.096130881077819363</v>
       </c>
       <c r="D4" s="0">
         <v>0.017280858673822157</v>
       </c>
       <c r="E4" s="0">
-        <v>0.54125243311192917</v>
+        <v>1.0226871836066638</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="0">
-        <v>0.16359563401046912</v>
+        <v>0.163590003978204</v>
       </c>
       <c r="C5" s="0">
         <v>0.096130881077819363</v>
@@ -1598,21 +1598,21 @@
     </row>
     <row r="6">
       <c r="B6" s="0">
-        <v>0.16541521325680167</v>
+        <v>0.16600584486135542</v>
       </c>
       <c r="C6" s="0">
-        <v>0.093354133549561638</v>
+        <v>0.094000978317784367</v>
       </c>
       <c r="D6" s="0">
         <v>0.020833333333333332</v>
       </c>
       <c r="E6" s="0">
-        <v>0.77948996279520577</v>
+        <v>0.77689778643548657</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="0">
-        <v>0.15694778429637588</v>
+        <v>0.18586072681643814</v>
       </c>
       <c r="C7" s="0">
         <v>0.10312517210071119</v>
@@ -1621,68 +1621,68 @@
         <v>0.022279520730885682</v>
       </c>
       <c r="E7" s="0">
-        <v>0.69546403423237346</v>
+        <v>1.615081120468761</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="0">
-        <v>0.1503037315795698</v>
+        <v>0.1488776818779258</v>
       </c>
       <c r="C8" s="0">
-        <v>0.11193492463045618</v>
+        <v>0.1119349351913262</v>
       </c>
       <c r="D8" s="0">
         <v>0.020833333333333332</v>
       </c>
       <c r="E8" s="0">
-        <v>0.74416484846224062</v>
+        <v>0.66328655993252106</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="0">
-        <v>0.17242133354815919</v>
+        <v>0.19332668151474214</v>
       </c>
       <c r="C9" s="0">
-        <v>0.11884108148540522</v>
+        <v>0.11916376021004907</v>
       </c>
       <c r="D9" s="0">
         <v>0.017280858673822182</v>
       </c>
       <c r="E9" s="0">
-        <v>1.243793887132292</v>
+        <v>1.617125535046023</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" s="0">
-        <v>0.19306443232346318</v>
+        <v>0.20611385872866034</v>
       </c>
       <c r="C10" s="0">
-        <v>0.11946201330855749</v>
+        <v>0.1210702795900534</v>
       </c>
       <c r="D10" s="0">
         <v>0.017280858673822182</v>
       </c>
       <c r="E10" s="0">
-        <v>0.66597361961715518</v>
+        <v>0.7289183994699544</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" s="0">
-        <v>0.17941225343353259</v>
+        <v>0.18975240438724972</v>
       </c>
       <c r="C11" s="0">
-        <v>0.11420721629833394</v>
+        <v>0.11148906885129026</v>
       </c>
       <c r="D11" s="0">
         <v>0.020833333333333332</v>
       </c>
       <c r="E11" s="0">
-        <v>0.8631039792230637</v>
+        <v>1.5453288837805428</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" s="0">
-        <v>0.15821989863103009</v>
+        <v>0.15817993262655128</v>
       </c>
       <c r="C12" s="0">
         <v>0.09613088107781935</v>
@@ -1691,12 +1691,12 @@
         <v>0.020833333333333332</v>
       </c>
       <c r="E12" s="0">
-        <v>1.2899957437060383</v>
+        <v>1.2952184210102733</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" s="0">
-        <v>0.12582089684408426</v>
+        <v>0.1259311121314666</v>
       </c>
       <c r="C13" s="0">
         <v>0.09118926714560352</v>
@@ -1705,12 +1705,12 @@
         <v>0.020319870679842908</v>
       </c>
       <c r="E13" s="0">
-        <v>0.56751632582875167</v>
+        <v>0.56834484299765931</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" s="0">
-        <v>0.13850155600274092</v>
+        <v>0.13849145187131001</v>
       </c>
       <c r="C14" s="0">
         <v>0.11826997444958734</v>
@@ -1719,7 +1719,7 @@
         <v>0.01728085867382223</v>
       </c>
       <c r="E14" s="0">
-        <v>0.61574813739659173</v>
+        <v>0.61334327247132925</v>
       </c>
     </row>
   </sheetData>
@@ -1732,7 +1732,7 @@
   <sheetData>
     <row r="2">
       <c r="B2" s="0">
-        <v>0.19678992339209334</v>
+        <v>0.19687802668961099</v>
       </c>
       <c r="C2" s="0">
         <v>0.13941234950789386</v>
@@ -1741,12 +1741,12 @@
         <v>0.034088984228514363</v>
       </c>
       <c r="E2" s="0">
-        <v>0.83951337066241127</v>
+        <v>0.83818385210135604</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" s="0">
-        <v>0.19959959394087459</v>
+        <v>0.19972659417788868</v>
       </c>
       <c r="C3" s="0">
         <v>0.13164541829057752</v>
@@ -1755,12 +1755,12 @@
         <v>0.029492985712615889</v>
       </c>
       <c r="E3" s="0">
-        <v>1.1186955642274643</v>
+        <v>1.1186097311464294</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="0">
-        <v>0.22710493568947482</v>
+        <v>0.22704290445130584</v>
       </c>
       <c r="C4" s="0">
         <v>0.13935924312167314</v>
@@ -1769,12 +1769,12 @@
         <v>0.034088984228514266</v>
       </c>
       <c r="E4" s="0">
-        <v>1.2377108392957181</v>
+        <v>1.2112333060003482</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="0">
-        <v>0.24361145984216234</v>
+        <v>0.24295315558359293</v>
       </c>
       <c r="C5" s="0">
         <v>0.1689451272523535</v>
@@ -1783,12 +1783,12 @@
         <v>0.036445961547596349</v>
       </c>
       <c r="E5" s="0">
-        <v>1.335618678324928</v>
+        <v>1.3382648913366397</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" s="0">
-        <v>0.24533191680863356</v>
+        <v>0.24537026963725647</v>
       </c>
       <c r="C6" s="0">
         <v>0.15266724273720433</v>
@@ -1797,54 +1797,54 @@
         <v>0.033299363131445645</v>
       </c>
       <c r="E6" s="0">
-        <v>1.3435131945060323</v>
+        <v>1.3469303760142375</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="0">
-        <v>0.23551762896667061</v>
+        <v>0.23420015043526951</v>
       </c>
       <c r="C7" s="0">
-        <v>0.17792858319531957</v>
+        <v>0.17492019893293365</v>
       </c>
       <c r="D7" s="0">
         <v>0.034088984228514363</v>
       </c>
       <c r="E7" s="0">
-        <v>1.2670650553975231</v>
+        <v>1.2611125990134333</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="0">
-        <v>0.21719649005096839</v>
+        <v>0.21881672459617113</v>
       </c>
       <c r="C8" s="0">
-        <v>0.15266147179761425</v>
+        <v>0.15258502010369734</v>
       </c>
       <c r="D8" s="0">
         <v>0.034088984228514266</v>
       </c>
       <c r="E8" s="0">
-        <v>1.2014445143046428</v>
+        <v>1.2115915528447039</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="0">
-        <v>0.24395494786764324</v>
+        <v>0.25430498572393695</v>
       </c>
       <c r="C9" s="0">
-        <v>0.18089800617224625</v>
+        <v>0.19530095871822661</v>
       </c>
       <c r="D9" s="0">
         <v>0.028548334230126409</v>
       </c>
       <c r="E9" s="0">
-        <v>1.579939586542991</v>
+        <v>1.5911816080227548</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" s="0">
-        <v>0.27889783279493036</v>
+        <v>0.27871394186979498</v>
       </c>
       <c r="C10" s="0">
         <v>0.22125822320691532</v>
@@ -1853,12 +1853,12 @@
         <v>0.028548334230126409</v>
       </c>
       <c r="E10" s="0">
-        <v>1.2500834992909435</v>
+        <v>1.2560567311256188</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" s="0">
-        <v>0.26384476923711392</v>
+        <v>0.2638151303342125</v>
       </c>
       <c r="C11" s="0">
         <v>0.18414950953877945</v>
@@ -1867,12 +1867,12 @@
         <v>0.027747933524242912</v>
       </c>
       <c r="E11" s="0">
-        <v>1.4503279627010266</v>
+        <v>1.4348229491854274</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" s="0">
-        <v>0.27243017153946236</v>
+        <v>0.27267650421731227</v>
       </c>
       <c r="C12" s="0">
         <v>0.19274363275060385</v>
@@ -1881,12 +1881,12 @@
         <v>0.034088984228514266</v>
       </c>
       <c r="E12" s="0">
-        <v>1.4418443355095729</v>
+        <v>1.4349618225817915</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" s="0">
-        <v>0.24964597647643991</v>
+        <v>0.24978103609460148</v>
       </c>
       <c r="C13" s="0">
         <v>0.16552810127353879</v>
@@ -1895,12 +1895,12 @@
         <v>0.034088984228514169</v>
       </c>
       <c r="E13" s="0">
-        <v>1.3136937736957031</v>
+        <v>1.3368341018485699</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" s="0">
-        <v>0.27264446484815119</v>
+        <v>0.27289998117570796</v>
       </c>
       <c r="C14" s="0">
         <v>0.14631321714489373</v>
@@ -1909,7 +1909,7 @@
         <v>0.034088984228514169</v>
       </c>
       <c r="E14" s="0">
-        <v>1.3195287580286226</v>
+        <v>1.3262869354489517</v>
       </c>
     </row>
   </sheetData>
@@ -1922,7 +1922,7 @@
   <sheetData>
     <row r="2">
       <c r="B2" s="0">
-        <v>0.13961530018900548</v>
+        <v>0.1462971562860661</v>
       </c>
       <c r="C2" s="0">
         <v>0.09191867997209538</v>
@@ -1931,40 +1931,40 @@
         <v>0.020833333333333332</v>
       </c>
       <c r="E2" s="0">
-        <v>0.78305773851557903</v>
+        <v>1.0486186781611722</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" s="0">
-        <v>0.13790754015775319</v>
+        <v>0.14452041641759397</v>
       </c>
       <c r="C3" s="0">
-        <v>0.09191867997209538</v>
+        <v>0.093780416278408607</v>
       </c>
       <c r="D3" s="0">
         <v>0.020833333333333332</v>
       </c>
       <c r="E3" s="0">
-        <v>0.72879055483770327</v>
+        <v>0.78147080350536846</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="0">
-        <v>0.14923826289891942</v>
+        <v>0.168350647558345</v>
       </c>
       <c r="C4" s="0">
-        <v>0.10312517210071119</v>
+        <v>0.10312750043327311</v>
       </c>
       <c r="D4" s="0">
         <v>0.017280858673822206</v>
       </c>
       <c r="E4" s="0">
-        <v>0.53451663864918508</v>
+        <v>1.2473298620279361</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="0">
-        <v>0.16336899790010823</v>
+        <v>0.17118898427466567</v>
       </c>
       <c r="C5" s="0">
         <v>0.096130881077819363</v>
@@ -1973,12 +1973,12 @@
         <v>0.022279520730885755</v>
       </c>
       <c r="E5" s="0">
-        <v>0.7469465770194369</v>
+        <v>0.76440030548387694</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" s="0">
-        <v>0.16104045416013463</v>
+        <v>0.16810541590918113</v>
       </c>
       <c r="C6" s="0">
         <v>0.09613088107781935</v>
@@ -1987,26 +1987,26 @@
         <v>0.020833333333333332</v>
       </c>
       <c r="E6" s="0">
-        <v>0.65376359927021876</v>
+        <v>0.72083841439344876</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="0">
-        <v>0.15297768451715305</v>
+        <v>0.16370338121232561</v>
       </c>
       <c r="C7" s="0">
-        <v>0.10312750043327311</v>
+        <v>0.10312982876583503</v>
       </c>
       <c r="D7" s="0">
         <v>0.01893334063186608</v>
       </c>
       <c r="E7" s="0">
-        <v>0.63041537653191881</v>
+        <v>0.88659469051963846</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="0">
-        <v>0.14389147924289308</v>
+        <v>0.14448361862955109</v>
       </c>
       <c r="C8" s="0">
         <v>0.11605026346086024</v>
@@ -2015,12 +2015,12 @@
         <v>0.020833333333333332</v>
       </c>
       <c r="E8" s="0">
-        <v>0.63017474195489698</v>
+        <v>0.62835688082535823</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="0">
-        <v>0.16295021085754496</v>
+        <v>0.16294964556434446</v>
       </c>
       <c r="C9" s="0">
         <v>0.13935924312167314</v>
@@ -2029,12 +2029,12 @@
         <v>0.020833333333333332</v>
       </c>
       <c r="E9" s="0">
-        <v>0.56098344348560736</v>
+        <v>0.5668123304628705</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" s="0">
-        <v>0.1989136182771892</v>
+        <v>0.19937073960991403</v>
       </c>
       <c r="C10" s="0">
         <v>0.11870821269090771</v>
@@ -2043,26 +2043,26 @@
         <v>0.020833333333333332</v>
       </c>
       <c r="E10" s="0">
-        <v>0.88235028922406034</v>
+        <v>0.86936556407631427</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" s="0">
-        <v>0.17490603593097878</v>
+        <v>0.19871975979209067</v>
       </c>
       <c r="C11" s="0">
-        <v>0.11420721629833394</v>
+        <v>0.11514760117446876</v>
       </c>
       <c r="D11" s="0">
         <v>0.019034719366727518</v>
       </c>
       <c r="E11" s="0">
-        <v>0.69208320058988959</v>
+        <v>1.783882803258616</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" s="0">
-        <v>0.15182938967342588</v>
+        <v>0.18016441999504684</v>
       </c>
       <c r="C12" s="0">
         <v>0.1236972157728071</v>
@@ -2071,12 +2071,12 @@
         <v>0.020833333333333332</v>
       </c>
       <c r="E12" s="0">
-        <v>0.56749872909504129</v>
+        <v>1.2952184210102733</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" s="0">
-        <v>0.13258031159468367</v>
+        <v>0.13255699981616675</v>
       </c>
       <c r="C13" s="0">
         <v>0.09613088107781935</v>
@@ -2085,12 +2085,12 @@
         <v>0.024184727847835503</v>
       </c>
       <c r="E13" s="0">
-        <v>0.53191901179927259</v>
+        <v>0.53166643421866189</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" s="0">
-        <v>0.14080395863491854</v>
+        <v>0.14073508913717403</v>
       </c>
       <c r="C14" s="0">
         <v>0.11216780416125958</v>
@@ -2099,7 +2099,7 @@
         <v>0.01728085867382223</v>
       </c>
       <c r="E14" s="0">
-        <v>0.53751698518260338</v>
+        <v>0.53954315811809717</v>
       </c>
     </row>
   </sheetData>

</xml_diff>